<commit_message>
feat: highlight current section on timeline
</commit_message>
<xml_diff>
--- a/data/shape.xlsx
+++ b/data/shape.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yiqiling/Documents/GitHub/bronze-clocks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E329A336-79E7-A045-BCC2-B02559924EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8F1344-CE97-0E4A-A36F-62AFA903F77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8140" yWindow="2840" windowWidth="27840" windowHeight="16940" xr2:uid="{1D9A6ED8-3B77-C843-AA98-28C755C818F3}"/>
+    <workbookView xWindow="1200" yWindow="1540" windowWidth="27840" windowHeight="16940" xr2:uid="{1D9A6ED8-3B77-C843-AA98-28C755C818F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -504,7 +504,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -538,7 +538,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -552,7 +552,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>

</xml_diff>